<commit_message>
PCB and DOCS update: Page structure (WIP) and BOM
</commit_message>
<xml_diff>
--- a/- DOCS -/Excel - COMPONENTS/aktuální seznam.xlsx
+++ b/- DOCS -/Excel - COMPONENTS/aktuální seznam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\OneDrive\Изображения\Документы\GitHub\RoboCop\- DOCS -\Excel - COMPONENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C42839A-7A0B-4C59-9929-7C7A769BE7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05BB14D-0728-4668-8A31-E677BA10E61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB5F3192-D3E9-42B8-A9EB-F1F11AD6B5B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>H most</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Konektro na Bat. 9V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vložky M3 </t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -662,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -841,7 +844,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -920,8 +923,12 @@
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="2">
+        <v>30</v>
+      </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>